<commit_message>
creation page app streamlit
</commit_message>
<xml_diff>
--- a/Passes avant un but/moy_passe_but.xlsx
+++ b/Passes avant un but/moy_passe_but.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,12 +453,66 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
+          <t>2023_2024</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>5.71578947368421</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4.960815047021944</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5.193932827735645</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2022_2023</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5.194331983805668</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5.136150234741784</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5.152370203160271</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2021_2022</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5.602076124567474</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4.869257950530035</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5.116959064327485</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
           <t>2020_2021</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="B5" t="n">
+        <v>4.778156996587031</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4.640138408304498</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4.686567164179104</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>